<commit_message>
series to list. opening function.
</commit_message>
<xml_diff>
--- a/add_data.xlsx
+++ b/add_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yello\Documents\GitHub\SheCodes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AFB1217-3FE1-4D05-B341-EB8EDA448F92}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD6BD965-F2B7-49EA-9D6E-0E9A2DA14619}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>Full Name</t>
   </si>
@@ -42,23 +42,32 @@
     <t>Hannah Owens</t>
   </si>
   <si>
-    <t>Job Title</t>
-  </si>
-  <si>
     <t>General Manager</t>
   </si>
   <si>
     <t>Martin Zess</t>
   </si>
   <si>
-    <t>Python Coordinator</t>
+    <t>Coordinator</t>
+  </si>
+  <si>
+    <t>Programming Languages</t>
+  </si>
+  <si>
+    <t>Python</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Python, JavaScript</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -67,6 +76,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -93,9 +109,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
@@ -378,10 +397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="E1" sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.35"/>
@@ -394,21 +413,24 @@
     <col min="6" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" ht="28" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>5</v>
+      <c r="D1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>214840</v>
       </c>
@@ -419,21 +441,27 @@
         <v>2</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>443346</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>